<commit_message>
update file Toi uu hoa du lieu.xlsx
</commit_message>
<xml_diff>
--- a/Toi uu hoa du lieu.xlsx
+++ b/Toi uu hoa du lieu.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\thuebannhadat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>- Chọn kiểu dữ liệu nhỏ hơn mà vẫn đáp ứng nhu cầu: vì chúng sử dụng ít bộ nhớ hơn, ít cache hơn</t>
     <phoneticPr fontId="1"/>
@@ -110,30 +110,612 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Vì những toán tử này nó không sử dụng đặc tính index mà thay vì thế nó sẽ dò tìm toàn bảng gây ảnh hưởng đến tốc độ của câu truy vấn. Ví dụ:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thay vì thế, bạn nên sử dụng </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT lname, fname, address FROM Customers WHERE fname LIKE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>‘%V%’</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT lname, fname, address FROM Customers WHERE fname LIKE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>‘V%’</t>
+    </r>
+  </si>
+  <si>
+    <t>- Nếu bạn có sự chọn lựa giữa IN và EXISTS trong câu truy vấn, bạn hãy chọn EXISTS là tốt nhất. Tương tự như IN và BETWEEN, hãy chọn BETWEEN</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Nên sử dụng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> trong câu lệnh </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> để thu hẹp số dòng trả về</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Không nên sử dụng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SELECT *</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- Cố gắng tránh sử dụng các toán tử sau trong mệnh đề WHERE: "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>IS NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>!=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>!&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>!&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NOT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NOT EXISTS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NOT IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NOT LIKE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>", and "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>LIKE '%abc'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT employeeID, firstname, lastname</t>
+  </si>
+  <si>
+    <t>FROM Employees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHERE dept = 'prod' or city = 'Orlando' or division = 'food' </t>
+  </si>
+  <si>
+    <t>Câu truy vấn sau cùng mục đích nhưng có tốc độ nhanh hơn</t>
+  </si>
+  <si>
+    <t>SELECT employeeID, firstname, lastname FROM Employees WHERE dept = 'prod'</t>
+  </si>
+  <si>
+    <t>UNION ALL</t>
+  </si>
+  <si>
+    <t>SELECT employeeID, firstname, lastname FROM Employees WHERE city = 'Orlando'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT employeeID, firstname, lastname FROM Employees WHERE division = 'food' </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Trong các câu truy vấn có 1/nhiều </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bạn có thể viết lại bằng cách kết hợp </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>UNION ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> để tăng tốc độ truy vấn</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Đừng sử dụng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>DISTINCT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> và </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ORDER BY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> trong câu lệnh </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> trừ khi thật sự cần thiết đến chúng vì chúng làm tăng chi phí xử lý câu truy vấn</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Nếu câu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> của bạn có sử dụng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>HAVING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bạn nên có thêm việc sử dụng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> để hạn chế những hàng không cần thiết</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT … WHERE … GROUP BY … HAVING ….</t>
+  </si>
+  <si>
+    <t>- Nên sử dụng IF EXISTS thay vì sử dụng COUNT(*) để xác định sự tồn tại của record trong bảng</t>
+  </si>
+  <si>
+    <t>IF (SELECT COUNT(*) FROM table_name WHERE column_name = 'xxx')</t>
+  </si>
+  <si>
+    <t>Hãy sử dụng IF EXISTS sẽ nhanh hơn:</t>
+  </si>
+  <si>
+    <t>IF EXISTS (SELECT * FROM table_name WHERE column_name = 'xxx')</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Sử dụng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>EXPLAIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> để tối ưu câu lệnh MySQL</t>
+    </r>
+  </si>
+  <si>
+    <t>https://viblo.asia/dinhhoanglong91/posts/BYjv44gmvxpV</t>
+  </si>
+  <si>
     <t>- DATETIME: hỗ trợ kiểu ký tự ngày giờ, mất 8 byte lưu trữ</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
   </si>
   <si>
     <t>- TIMESTAMP: mất 4 byte lưu trữ</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>MEDIUMINT</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Khai báo cột là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NOT NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> nếu có thể. Bạn cũng tiết kiệm được một chút không gian lưu trữ, một bit cho mỗi cột</t>
+    </r>
+  </si>
+  <si>
+    <t>INT(2)</t>
+  </si>
+  <si>
+    <t>TINYINT</t>
+  </si>
+  <si>
+    <t>=&gt;</t>
+  </si>
+  <si>
+    <t>VARCHAR (MD5)</t>
+  </si>
+  <si>
+    <t>CHAR</t>
+  </si>
+  <si>
+    <t>tên, địa chỉ,...</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -148,7 +730,45 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -179,7 +799,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -189,7 +809,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -208,6 +834,65 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Arrow 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6088380" y="2247900"/>
+          <a:ext cx="937260" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,46 +1158,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:16">
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:16">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:16">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:16">
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:16">
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
@@ -520,7 +1205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:16">
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
@@ -531,7 +1216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:16">
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
@@ -542,7 +1227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:16">
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
@@ -553,50 +1238,237 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="11" spans="1:16">
+      <c r="M11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="M12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="M13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="M14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="M15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="3:3">
+    <row r="17" spans="2:3">
       <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
       <c r="C18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
       <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="2:3">
       <c r="C20" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="C21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="16.2">
+      <c r="C27" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="C28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="16.2">
+      <c r="C29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="16.2">
+      <c r="C32" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="16.2">
+      <c r="C33" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="16.2">
+      <c r="C34" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="C35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="16.2">
+      <c r="C36" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="16.2">
+      <c r="C37" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="16.2">
+      <c r="C38" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="16.2">
+      <c r="C39" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="16.2">
+      <c r="C40" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="16.2">
+      <c r="C44" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="16.2">
+      <c r="C46" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="C47" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="16.2">
+      <c r="C48" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="C50" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -605,5 +1477,7 @@
     <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>